<commit_message>
Update Persentase Penduduk Miskin (P0) Menurut Provinsi dan Daerah, 2020.xlsx
</commit_message>
<xml_diff>
--- a/p0-persentase-penduduk-miskin/Persentase Penduduk Miskin (P0) Menurut Provinsi dan Daerah, 2020.xlsx
+++ b/p0-persentase-penduduk-miskin/Persentase Penduduk Miskin (P0) Menurut Provinsi dan Daerah, 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/dhiya_muharram_binus_ac_id/Documents/0. Lomba &amp; Sertifikat Dokum/Data Slayer/Github/dataset-slayer/p0-persentase-penduduk-miskin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_40EF431F97E9BB65426102AB8855B237A12C5022" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10925C06-6F88-4CFE-ACE8-EA21DE3D4F5F}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_40EF431F97E9BB65426102AB8855B237A12C5022" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A072FDE-9EF3-4F8E-9BA9-A375E6EE6C4F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,13 +557,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" activeCellId="1" sqref="C6 F6"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
@@ -571,12 +571,12 @@
     <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -590,7 +590,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -608,7 +608,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>2020</v>
@@ -626,7 +626,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>5</v>
@@ -656,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -687,12 +687,8 @@
       <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="K6">
-        <f>AVERAGE(B6,E6)</f>
-        <v>13.65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -724,7 +720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -756,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -788,7 +784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -820,7 +816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -852,7 +848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -884,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -916,7 +912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -948,7 +944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -980,7 +976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1012,7 +1008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1044,7 +1040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1076,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1172,7 +1168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1204,7 +1200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1236,7 +1232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1300,7 +1296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1332,7 +1328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1364,7 +1360,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1396,7 +1392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1428,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1460,7 +1456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1492,7 +1488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1588,7 +1584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1620,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1652,7 +1648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1684,7 +1680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1716,7 +1712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1748,7 +1744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1780,7 +1776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1812,7 +1808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1844,7 +1840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1876,7 +1872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>47</v>
       </c>

</xml_diff>